<commit_message>
spezifikatinen immer noch nicht fehlerfrei
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-cde-blood-pressure-diastolic.xlsx
+++ b/output/StructureDefinition-cde-blood-pressure-diastolic.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-03-06T16:38:28+01:00</t>
+    <t>2023-03-06T17:18:53+01:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -84,7 +84,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Dieses CDE enthät den 'systolischen Blutdruck'.</t>
+    <t>Dieses CDE enthät den 'diastolischen Blutdruck'.</t>
   </si>
   <si>
     <t>Purpose</t>
@@ -114,7 +114,7 @@
     <t>Base Definition</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/StructureDefinition/Observation</t>
+    <t>http://somewhere.org/fhir/uv/myig/StructureDefinition/cls-obo-cmo-diastolic-blood-pressure</t>
   </si>
   <si>
     <t>Abstract</t>

</xml_diff>